<commit_message>
inclusão de linhas nos arquivos em excel para Vendas_Consolidado
</commit_message>
<xml_diff>
--- a/ETL/ArquivosExcel/Vendas2023.xlsx
+++ b/ETL/ArquivosExcel/Vendas2023.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmil\OneDrive\Área de Trabalho\Python\Arquivos\Origem\arquivos_excel\Consolidar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\ETL\ArquivosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1F32A8-4884-496E-A01F-2DA76DF5BD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Data</t>
   </si>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -166,7 +167,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{ADA0A52F-643E-4DF4-AA26-4031B93D32E5}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -462,11 +465,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,6 +887,47 @@
         <v>2959.2</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B11">
+        <v>394</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>639</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11">
+        <v>250</v>
+      </c>
+      <c r="J11">
+        <v>290</v>
+      </c>
+      <c r="K11">
+        <v>300</v>
+      </c>
+      <c r="L11">
+        <v>87000</v>
+      </c>
+      <c r="M11">
+        <v>19392</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>